<commit_message>
"maintain Core elements files"
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Youxel\Check Automation\CheckPlus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Al Riyadh Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A807AA8-42D2-486D-9765-57FF63F590FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2C9E1F-9C42-49AE-969F-D6877D0C5EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>faker reader</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>highlight all elements</t>
   </si>
@@ -36,10 +33,31 @@
     <t>error screenshoot</t>
   </si>
   <si>
-    <t xml:space="preserve">el 7aga elly 3nd sleem f el shat </t>
-  </si>
-  <si>
-    <t>deal with alert  while toggle activation</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>read from json file</t>
+  </si>
+  <si>
+    <t>maintaine all files</t>
+  </si>
+  <si>
+    <t>in pregress</t>
+  </si>
+  <si>
+    <t>UML Class diagram for the project structure</t>
+  </si>
+  <si>
+    <t>doc for all files</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>redmi file</t>
+  </si>
+  <si>
+    <t>TO DO</t>
   </si>
 </sst>
 </file>
@@ -64,7 +82,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -81,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -364,40 +383,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"maintain json file and submit report"
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Al Riyadh Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2C9E1F-9C42-49AE-969F-D6877D0C5EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9A8F2C-5C13-4E3B-8A56-883636383155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>highlight all elements</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>TO DO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate on the userName while login succeseded </t>
+  </si>
+  <si>
+    <t xml:space="preserve">make the validation of the report dinamically </t>
+  </si>
+  <si>
+    <t>use soft assert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the selected Municability, district, and street we can handle it by street name </t>
   </si>
 </sst>
 </file>
@@ -99,9 +111,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -383,15 +394,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.88671875" customWidth="1"/>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
     <col min="2" max="2" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -404,31 +415,31 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -449,6 +460,38 @@
       </c>
       <c r="B7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>